<commit_message>
work fixing to placement system
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -64,18 +64,36 @@
   <si>
     <t>Time allocated</t>
   </si>
+  <si>
+    <t>Time (h)</t>
+  </si>
+  <si>
+    <t>Started bug fixing and writing more functionality to fit my requirtements</t>
+  </si>
+  <si>
+    <t>Started bug fixing and writing more functionality to fit my requirtements. Also fixed all of the ship prefabs and implemented a simple UI system.</t>
+  </si>
+  <si>
+    <t>Placing ships still glitchy. Think its to do with colliders.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -92,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,14 +135,37 @@
         <color rgb="FF000000"/>
       </diagonal>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="16" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment wrapText="1" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,14 +484,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="67.85546875" customWidth="1"/>
-    <col min="5" max="5" width="136.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" customWidth="1" style="3"/>
+    <col min="5" max="5" width="136.7109375" customWidth="1" style="3"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -467,7 +508,7 @@
       </c>
       <c r="C3">
         <f>SUM(C7:C39)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -476,7 +517,7 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
@@ -484,12 +525,12 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -500,10 +541,10 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -514,11 +555,25 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" ht="28">
+      <c r="B9" s="2">
+        <v>45348</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref timelog for notes
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Day</t>
   </si>
@@ -98,13 +98,25 @@
   </si>
   <si>
     <t>Need a lot more work to find neighbours and then get the link to the player action script to get the values of there ships</t>
+  </si>
+  <si>
+    <t>Added a bounding box for map</t>
+  </si>
+  <si>
+    <t>Added a bounding box for map. Fixed prefab sizes and hit boxes.</t>
+  </si>
+  <si>
+    <t>Added a bounding box for map. Fixed prefab sizes and hit boxes. Created dictionary for all tiles</t>
+  </si>
+  <si>
+    <t>Dictionary created. Need to create one for finding out where player ship placements are and then can link to attacking script.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +154,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -194,11 +212,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -213,6 +248,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,17 +569,17 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D17" sqref="D17" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="67.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="136.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -549,25 +587,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
         <f>SUM(C7:C39)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -581,7 +619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="B7" s="1">
         <v>45346</v>
       </c>
@@ -595,7 +633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="B8" s="1">
         <v>45347</v>
       </c>
@@ -609,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" ht="30">
       <c r="B9" s="2">
         <v>45348</v>
       </c>
@@ -623,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="B10" s="4">
         <v>45349</v>
       </c>
@@ -637,7 +675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="B11" s="5">
         <v>45352</v>
       </c>
@@ -651,7 +689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="B12" s="6">
         <v>45353</v>
       </c>
@@ -665,7 +703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="B13" s="8">
         <v>45364</v>
       </c>
@@ -677,6 +715,20 @@
       </c>
       <c r="E13" s="10" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="14" ht="28">
+      <c r="B14" s="11">
+        <v>45365</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +742,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -702,7 +754,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added assets and fonts to game
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -120,12 +120,33 @@
   <si>
     <t>AI can now know when it hits a ship. It can find the neighbours of that tile. Need to make sure that AI knows which its has already chosen so it doesnt repeat choices.</t>
   </si>
+  <si>
+    <t>Found more assets and a font to usew in the game</t>
+  </si>
+  <si>
+    <t>Added assets and font to game.</t>
+  </si>
+  <si>
+    <t>Found more assets and a font to use in the game</t>
+  </si>
+  <si>
+    <t>Added assets and font to game. Made game look good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Still need to fix the AI player then work on the players attactks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Still need to fix the AI then work on the players attactks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collision with missle wont work. Still need to fix the AI then work on the players attacks, finally think about having a second map that shows the player where they have hit more miss to increase playablity like in real battleships. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +200,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <family val="2"/>
     </font>
     <font>
@@ -196,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -277,11 +304,28 @@
         <color rgb="FF000000"/>
       </diagonal>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -301,6 +345,9 @@
     <xf numFmtId="16" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="9" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="16" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="10" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -620,7 +667,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19" activeCellId="0"/>
+      <selection activeCell="E22" sqref="E22" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -644,7 +691,7 @@
       </c>
       <c r="C3">
         <f>SUM(C7:C39)</f>
-        <v>24.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="4">
@@ -653,7 +700,7 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>17.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="6">
@@ -824,7 +871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" ht="28">
+    <row r="18" ht="27">
       <c r="B18" s="14">
         <v>45372</v>
       </c>
@@ -836,6 +883,31 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="15">
+        <v>45373</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" ht="28">
+      <c r="B20" s="15">
+        <v>45374</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>